<commit_message>
update max, mini. close
</commit_message>
<xml_diff>
--- a/giaothong/bin/Debug/dsxetaplai.xlsx
+++ b/giaothong/bin/Debug/dsxetaplai.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>TRƯỜNG CAO ĐẲNG CĐ-XD&amp;NL</t>
   </si>
@@ -69,6 +69,9 @@
   </si>
   <si>
     <t xml:space="preserve">SDK001    </t>
+  </si>
+  <si>
+    <t>X</t>
   </si>
   <si>
     <t xml:space="preserve">Toyota         </t>
@@ -123,7 +126,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="&quot;Ngày&quot; dd&quot; tháng &quot;MM&quot; năm &quot;yyyy"/>
+  </numFmts>
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -154,7 +159,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -163,6 +168,13 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin"/>
       <right style="thin"/>
       <top style="thin"/>
@@ -177,6 +189,13 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right style="thin"/>
       <top/>
@@ -187,7 +206,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" xfId="0" applyAlignment="1">
@@ -199,9 +218,15 @@
     <xf numFmtId="0" fontId="2" applyFont="1" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" applyFill="1" borderId="1" applyBorder="1" xfId="0"/>
-    <xf numFmtId="0" fontId="0" borderId="2" applyBorder="1" xfId="0"/>
+    <xf numFmtId="0" fontId="1" applyFont="1" xfId="0"/>
     <xf numFmtId="0" fontId="0" borderId="3" applyBorder="1" xfId="0"/>
+    <xf numFmtId="0" fontId="0" borderId="4" applyBorder="1" xfId="0"/>
+    <xf numFmtId="0" fontId="1" applyFont="1" fillId="2" applyFill="1" borderId="2" applyBorder="1" xfId="0"/>
+    <xf numFmtId="0" fontId="0" borderId="5" applyBorder="1" xfId="0"/>
+    <xf numFmtId="0" fontId="0" borderId="1" applyBorder="1" xfId="0"/>
+    <xf numFmtId="164" applyNumberFormat="1" fontId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -219,18 +244,20 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.140625" customWidth="1" style="1"/>
-    <col min="2" max="2" width="25" customWidth="1" style="1"/>
-    <col min="3" max="3" width="15" customWidth="1" style="1"/>
-    <col min="4" max="4" width="15" customWidth="1" style="1"/>
-    <col min="5" max="5" width="15" customWidth="1" style="1"/>
-    <col min="6" max="6" width="15" customWidth="1" style="1"/>
-    <col min="7" max="7" width="13" customWidth="1" style="1"/>
-    <col min="8" max="8" width="13" customWidth="1" style="1"/>
-    <col min="9" max="9" width="13" customWidth="1" style="1"/>
-    <col min="10" max="10" width="15" customWidth="1" style="1"/>
-    <col min="11" max="11" width="15" customWidth="1" style="1"/>
-    <col min="12" max="12" width="25" customWidth="1" style="1"/>
-    <col min="13" max="16384" width="9.140625" customWidth="1" style="1"/>
+    <col min="2" max="2" width="28.764162336077" customWidth="1" style="1"/>
+    <col min="3" max="3" width="12.2007359095982" customWidth="1" style="1"/>
+    <col min="4" max="4" width="13.5982426234654" customWidth="1" style="1"/>
+    <col min="5" max="5" width="9.92134639195034" customWidth="1" style="1"/>
+    <col min="6" max="6" width="9.140625" customWidth="1" style="1"/>
+    <col min="7" max="7" width="9.140625" customWidth="1" style="1"/>
+    <col min="8" max="8" width="13.0038419451032" customWidth="1" style="1"/>
+    <col min="9" max="9" width="14.2182203020368" customWidth="1" style="1"/>
+    <col min="10" max="10" width="67.7050999232701" customWidth="1" style="1"/>
+    <col min="11" max="11" width="38.0750819614955" customWidth="1" style="1"/>
+    <col min="12" max="12" width="9.140625" customWidth="1" style="1"/>
+    <col min="13" max="13" width="13.0089547293527" customWidth="1" style="1"/>
+    <col min="14" max="14" width="9.140625" customWidth="1" style="1"/>
+    <col min="15" max="16384" width="9.140625" customWidth="1" style="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -284,45 +311,46 @@
       <c r="M4" s="3"/>
     </row>
     <row r="5">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="H5" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="I5" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="J5" s="5" t="s">
+      <c r="J5" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="K5" s="5" t="s">
+      <c r="K5" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="L5" s="5" t="s">
+      <c r="L5" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="M5" s="5" t="s">
+      <c r="M5" s="8" t="s">
         <v>17</v>
       </c>
+      <c r="N5" s="5"/>
     </row>
     <row r="6">
       <c r="A6" s="6">
@@ -331,23 +359,20 @@
       <c r="B6" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="E6" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="F6" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="G6" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="H6" s="6" t="s">
         <v>23</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>24</v>
       </c>
       <c r="I6" s="6" t="s">
         <v>24</v>
@@ -356,47 +381,57 @@
         <v>25</v>
       </c>
       <c r="K6" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="L6" s="6" t="s">
         <v>26</v>
       </c>
+      <c r="M6" s="6" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="7">
-      <c r="A7" s="7">
+      <c r="A7" s="9">
         <v>2</v>
       </c>
-      <c r="B7" s="7" t="s">
-        <v>27</v>
+      <c r="B7" s="9" t="s">
+        <v>28</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E7" s="7" t="s">
+      <c r="D7" s="10"/>
+      <c r="E7" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="G7" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="H7" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="H7" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="I7" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="J7" s="7" t="s">
+      <c r="I7" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="J7" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="K7" s="6" t="s">
-        <v>32</v>
+      <c r="K7" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="L7" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="M7" s="9" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="8">
-      <c r="K8" s="2">
-        <v>45161.4089644792</v>
+      <c r="K8" s="11">
+        <v>45167.8431644444</v>
       </c>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
@@ -404,12 +439,12 @@
     </row>
     <row r="9">
       <c r="B9" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="K9" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>

</xml_diff>

<commit_message>
change code vehicle, teacher, combobox and fix bug
</commit_message>
<xml_diff>
--- a/giaothong/bin/Debug/dsxetaplai.xlsx
+++ b/giaothong/bin/Debug/dsxetaplai.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>TRƯỜNG CAO ĐẲNG CĐ-XD&amp;NL</t>
   </si>
@@ -68,7 +68,7 @@
     <t>Ghi chú</t>
   </si>
   <si>
-    <t xml:space="preserve">SDK001    </t>
+    <t xml:space="preserve">77B0999   </t>
   </si>
   <si>
     <t>X</t>
@@ -77,16 +77,10 @@
     <t xml:space="preserve">Toyota         </t>
   </si>
   <si>
-    <t xml:space="preserve">Xe con              </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018      </t>
-  </si>
-  <si>
-    <t>Xe t?i B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B1   </t>
+    <t xml:space="preserve">2023      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">B1 </t>
   </si>
   <si>
     <t>Tạm thời không có trong db</t>
@@ -95,25 +89,16 @@
     <t/>
   </si>
   <si>
-    <t xml:space="preserve">Quang Dat                     </t>
+    <t xml:space="preserve">Quang Ð?t                     </t>
   </si>
   <si>
     <t xml:space="preserve">SDK002    </t>
   </si>
   <si>
-    <t xml:space="preserve">Xe  Vip             </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023      </t>
-  </si>
-  <si>
-    <t>Mô tô</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A3   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ho Quang Dat                  </t>
+    <t xml:space="preserve">RR             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quoc Anh                      </t>
   </si>
   <si>
     <t>Hiệu trưởng</t>
@@ -255,7 +240,7 @@
     <col min="10" max="10" width="67.7050999232701" customWidth="1" style="1"/>
     <col min="11" max="11" width="38.0750819614955" customWidth="1" style="1"/>
     <col min="12" max="12" width="9.140625" customWidth="1" style="1"/>
-    <col min="13" max="13" width="13.0089547293527" customWidth="1" style="1"/>
+    <col min="13" max="13" width="10.0246734619141" customWidth="1" style="1"/>
     <col min="14" max="14" width="9.140625" customWidth="1" style="1"/>
     <col min="15" max="16384" width="9.140625" customWidth="1" style="1"/>
   </cols>
@@ -366,28 +351,28 @@
         <v>20</v>
       </c>
       <c r="F6" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="H6" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I6" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="J6" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="I6" s="6" t="s">
+      <c r="K6" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="L6" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="J6" s="6" t="s">
+      <c r="M6" s="6" t="s">
         <v>25</v>
-      </c>
-      <c r="K6" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="L6" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="M6" s="6" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="7">
@@ -395,43 +380,43 @@
         <v>2</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>19</v>
       </c>
       <c r="D7" s="10"/>
       <c r="E7" s="9" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="J7" s="9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="K7" s="9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="L7" s="9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="M7" s="9" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8">
       <c r="K8" s="11">
-        <v>45167.8431644444</v>
+        <v>45183.8613597222</v>
       </c>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
@@ -439,12 +424,12 @@
     </row>
     <row r="9">
       <c r="B9" s="3" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="K9" s="3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>

</xml_diff>